<commit_message>
completed Chapter 11 Running Case 2
</commit_message>
<xml_diff>
--- a/Ch11Rc02(PDQ)/Ch11Rc02(PDQ).xlsx
+++ b/Ch11Rc02(PDQ)/Ch11Rc02(PDQ).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Medium</t>
   </si>
@@ -25,6 +25,13 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>RISK 1
+RISK 2</t>
+  </si>
+  <si>
+    <t>RISK 3</t>
   </si>
 </sst>
 </file>
@@ -81,15 +88,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -162,7 +174,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>322008</xdr:colOff>
+      <xdr:colOff>464883</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>182817</xdr:rowOff>
     </xdr:from>
@@ -174,7 +186,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3408108" y="4745292"/>
+          <a:off x="4017708" y="5421567"/>
           <a:ext cx="1050416" cy="468013"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -272,11 +284,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>228598</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1619250" cy="609013"/>
+    <xdr:ext cx="4114801" cy="1409700"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -284,8 +296,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7696200" y="914400"/>
-          <a:ext cx="1619250" cy="609013"/>
+          <a:off x="7696198" y="914400"/>
+          <a:ext cx="4114801" cy="1409700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -308,7 +320,7 @@
       </xdr:style>
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
+          <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
@@ -319,12 +331,20 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1.</a:t>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>1. No Order Data</a:t>
           </a:r>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> </a:t>
+            <a:t>2. No Factory Data</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>3. Factory Locator Subsystem Server Down (centralized architecture)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -628,17 +648,17 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="26.25" style="3" customWidth="1"/>
-    <col min="4" max="4" width="25.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="25.75" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.125" style="3"/>
+    <col min="2" max="2" width="12.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.75" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -646,35 +666,39 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="2:5" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="2:5" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chnage chapter 11 task 1
</commit_message>
<xml_diff>
--- a/Ch11Rc02(PDQ)/Ch11Rc02(PDQ).xlsx
+++ b/Ch11Rc02(PDQ)/Ch11Rc02(PDQ).xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawei/Documents/School/Courses/Project Management/Repo/Project-Management-Year-4-Semister-1/Ch11Rc02(PDQ)/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19F8906-4C82-CF48-A212-D4096A8EFE35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="19020" windowHeight="8325"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Medium</t>
   </si>
@@ -33,11 +39,14 @@
   <si>
     <t>RISK 3</t>
   </si>
+  <si>
+    <t>RISK 4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -113,6 +122,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -129,7 +141,13 @@
     <xdr:ext cx="468013" cy="1538498"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -181,7 +199,13 @@
     <xdr:ext cx="1050416" cy="468013"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -233,7 +257,13 @@
     <xdr:ext cx="6419850" cy="843693"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -291,7 +321,13 @@
     <xdr:ext cx="4114801" cy="1409700"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -345,6 +381,12 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>3. Factory Locator Subsystem Server Down (centralized architecture)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>4. Training</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -401,7 +443,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -434,9 +476,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -469,6 +528,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -644,25 +720,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.75" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.125" style="2"/>
+    <col min="2" max="2" width="12.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:5" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:5" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -670,17 +745,19 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="2:5" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="117.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="2:5" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="117.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -690,7 +767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>2</v>
@@ -710,24 +787,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>